<commit_message>
Deleted old monthly mastersheet
</commit_message>
<xml_diff>
--- a/data/Monthly Mastersheet.xlsx
+++ b/data/Monthly Mastersheet.xlsx
@@ -1910,7 +1910,7 @@
         <v>0.01792743</v>
       </c>
       <c r="Z13" s="26">
-        <v>0.00334719</v>
+        <v>0.002881825</v>
       </c>
       <c r="AA13" s="26">
         <v>0.01237843</v>
@@ -1997,7 +1997,7 @@
         <v>0.01724086</v>
       </c>
       <c r="Z14" s="26">
-        <v>0.00242823</v>
+        <v>0.002907675</v>
       </c>
       <c r="AA14" s="26">
         <v>0.00668874</v>
@@ -2084,7 +2084,7 @@
         <v>0.01795248</v>
       </c>
       <c r="Z15" s="26">
-        <v>0.00242823</v>
+        <v>0.002311613</v>
       </c>
       <c r="AA15" s="26">
         <v>0.00668874</v>
@@ -2171,7 +2171,7 @@
         <v>0.02099296</v>
       </c>
       <c r="Z16" s="26">
-        <v>0.00242823</v>
+        <v>0.002260083</v>
       </c>
       <c r="AA16" s="26">
         <v>0.00668874</v>
@@ -2258,7 +2258,7 @@
         <v>0.02216797</v>
       </c>
       <c r="Z17" s="26">
-        <v>0.00209914</v>
+        <v>0.002536348</v>
       </c>
       <c r="AA17" s="26">
         <v>0.00619385</v>
@@ -2347,7 +2347,7 @@
         <v>0.0201725</v>
       </c>
       <c r="Z18" s="26">
-        <v>0.00209914</v>
+        <v>0.002658828</v>
       </c>
       <c r="AA18" s="26">
         <v>0.00619385</v>
@@ -2436,7 +2436,7 @@
         <v>0.01907862</v>
       </c>
       <c r="Z19" s="26">
-        <v>0.00209914</v>
+        <v>0.002352693</v>
       </c>
       <c r="AA19" s="26">
         <v>0.00619385</v>
@@ -2525,7 +2525,7 @@
         <v>0.02030439</v>
       </c>
       <c r="Z20" s="26">
-        <v>0.0026283</v>
+        <v>0.00238231</v>
       </c>
       <c r="AA20" s="26">
         <v>0.00672521</v>
@@ -2614,7 +2614,7 @@
         <v>0.01977953</v>
       </c>
       <c r="Z21" s="26">
-        <v>0.0026283</v>
+        <v>0.002200334</v>
       </c>
       <c r="AA21" s="26">
         <v>0.00672521</v>
@@ -2703,7 +2703,7 @@
         <v>0.0201923</v>
       </c>
       <c r="Z22" s="26">
-        <v>0.0026283</v>
+        <v>0.002503678</v>
       </c>
       <c r="AA22" s="26">
         <v>0.00672521</v>
@@ -2792,7 +2792,7 @@
         <v>0.02009312</v>
       </c>
       <c r="Z23" s="26">
-        <v>0.00356064</v>
+        <v>0.002609351</v>
       </c>
       <c r="AA23" s="26">
         <v>0.00682237</v>
@@ -2881,7 +2881,7 @@
         <v>0.02014402</v>
       </c>
       <c r="Z24" s="26">
-        <v>0.00356064</v>
+        <v>0.002615849</v>
       </c>
       <c r="AA24" s="26">
         <v>0.00682237</v>
@@ -2970,7 +2970,7 @@
         <v>0.02055907</v>
       </c>
       <c r="Z25" s="26">
-        <v>0.00356064</v>
+        <v>0.002441466</v>
       </c>
       <c r="AA25" s="26">
         <v>0.00682237</v>
@@ -3059,7 +3059,7 @@
         <v>0.02045245</v>
       </c>
       <c r="Z26" s="26">
-        <v>0.00363607</v>
+        <v>0.002389412</v>
       </c>
       <c r="AA26" s="26">
         <v>0.00873317</v>
@@ -3148,7 +3148,7 @@
         <v>0.0193736</v>
       </c>
       <c r="Z27" s="26">
-        <v>0.00363607</v>
+        <v>0.002558693</v>
       </c>
       <c r="AA27" s="26">
         <v>0.00873317</v>
@@ -3237,7 +3237,7 @@
         <v>0.01843703</v>
       </c>
       <c r="Z28" s="26">
-        <v>0.00363607</v>
+        <v>0.002664749</v>
       </c>
       <c r="AA28" s="26">
         <v>0.00873317</v>
@@ -3326,7 +3326,7 @@
         <v>0.0184505</v>
       </c>
       <c r="Z29" s="26">
-        <v>0.00606199</v>
+        <v>0.002760751</v>
       </c>
       <c r="AA29" s="26">
         <v>0.01374177</v>
@@ -3415,7 +3415,7 @@
         <v>0.01834828</v>
       </c>
       <c r="Z30" s="26">
-        <v>0.00606199</v>
+        <v>0.002344237</v>
       </c>
       <c r="AA30" s="26">
         <v>0.01374177</v>
@@ -3504,7 +3504,7 @@
         <v>0.02653112</v>
       </c>
       <c r="Z31" s="26">
-        <v>0.00606199</v>
+        <v>0.01527575</v>
       </c>
       <c r="AA31" s="26">
         <v>0.01374177</v>
@@ -3593,7 +3593,7 @@
         <v>0.04198924</v>
       </c>
       <c r="Z32" s="26">
-        <v>0.02465956</v>
+        <v>0.030582684</v>
       </c>
       <c r="AA32" s="26">
         <v>0.06282448</v>
@@ -3682,7 +3682,7 @@
         <v>0.34502209</v>
       </c>
       <c r="Z33" s="26">
-        <v>0.02465956</v>
+        <v>0.033921762</v>
       </c>
       <c r="AA33" s="26">
         <v>0.06282448</v>
@@ -3771,7 +3771,7 @@
         <v>0.34482623</v>
       </c>
       <c r="Z34" s="26">
-        <v>0.02465956</v>
+        <v>0.037371788</v>
       </c>
       <c r="AA34" s="26">
         <v>0.06282448</v>
@@ -3860,7 +3860,7 @@
         <v>0.34475186</v>
       </c>
       <c r="Z35" s="26">
-        <v>0.03402407</v>
+        <v>0.037987322</v>
       </c>
       <c r="AA35" s="26">
         <v>0.08546735</v>
@@ -3949,7 +3949,7 @@
         <v>0.34421615</v>
       </c>
       <c r="Z36" s="26">
-        <v>0.03402407</v>
+        <v>0.038079378</v>
       </c>
       <c r="AA36" s="26">
         <v>0.08546735</v>
@@ -4038,7 +4038,7 @@
         <v>0.34425563</v>
       </c>
       <c r="Z37" s="26">
-        <v>0.03402407</v>
+        <v>0.038221205</v>
       </c>
       <c r="AA37" s="26">
         <v>0.08546735</v>
@@ -4127,7 +4127,7 @@
         <v>0.34393652</v>
       </c>
       <c r="Z38" s="26">
-        <v>0.03414292</v>
+        <v>0.038265627</v>
       </c>
       <c r="AA38" s="26">
         <v>0.08884704</v>
@@ -4216,7 +4216,7 @@
         <v>0.34351906</v>
       </c>
       <c r="Z39" s="26">
-        <v>0.03414292</v>
+        <v>0.038315242</v>
       </c>
       <c r="AA39" s="26">
         <v>0.08884704</v>
@@ -4305,7 +4305,7 @@
         <v>0.3439417</v>
       </c>
       <c r="Z40" s="26">
-        <v>0.03414292</v>
+        <v>0.038390258</v>
       </c>
       <c r="AA40" s="26">
         <v>0.08884704</v>
@@ -4394,7 +4394,7 @@
         <v>0.34286314</v>
       </c>
       <c r="Z41" s="26">
-        <v>0.03408908</v>
+        <v>0.03867463</v>
       </c>
       <c r="AA41" s="26">
         <v>0.08892419</v>
@@ -4483,7 +4483,7 @@
         <v>0.34255764</v>
       </c>
       <c r="Z42" s="26">
-        <v>0.03408908</v>
+        <v>0.038905508</v>
       </c>
       <c r="AA42" s="26">
         <v>0.08892419</v>
@@ -4572,7 +4572,7 @@
         <v>0.34354265</v>
       </c>
       <c r="Z43" s="26">
-        <v>0.03408908</v>
+        <v>0.036090694</v>
       </c>
       <c r="AA43" s="26">
         <v>0.08892419</v>
@@ -4661,7 +4661,7 @@
         <v>0.34476236</v>
       </c>
       <c r="Z44" s="26">
-        <v>0.02142037</v>
+        <v>0.018279366</v>
       </c>
       <c r="AA44" s="26">
         <v>0.05335121</v>
@@ -4750,7 +4750,7 @@
         <v>0.00738706</v>
       </c>
       <c r="Z45" s="26">
-        <v>0.02142037</v>
+        <v>0.016241031</v>
       </c>
       <c r="AA45" s="26">
         <v>0.05335121</v>
@@ -4839,7 +4839,7 @@
         <v>0.0069325</v>
       </c>
       <c r="Z46" s="26">
-        <v>0.02142037</v>
+        <v>0.010846805</v>
       </c>
       <c r="AA46" s="26">
         <v>0.05335121</v>
@@ -4928,7 +4928,7 @@
         <v>0.00701931</v>
       </c>
       <c r="Z47" s="26">
-        <v>0.00601616</v>
+        <v>0.009705806</v>
       </c>
       <c r="AA47" s="26">
         <v>0.02756993</v>
@@ -5017,7 +5017,7 @@
         <v>0.00676105</v>
       </c>
       <c r="Z48" s="26">
-        <v>0.00601616</v>
+        <v>0.009742843</v>
       </c>
       <c r="AA48" s="26">
         <v>0.02756993</v>
@@ -5106,7 +5106,7 @@
         <v>0.00669713</v>
       </c>
       <c r="Z49" s="26">
-        <v>0.00601616</v>
+        <v>0.009538708</v>
       </c>
       <c r="AA49" s="26">
         <v>0.02756993</v>
@@ -5195,7 +5195,7 @@
         <v>0.00673594</v>
       </c>
       <c r="Z50" s="26">
-        <v>0.00682379</v>
+        <v>0.009846431</v>
       </c>
       <c r="AA50" s="26">
         <v>0.0249992</v>
@@ -5284,7 +5284,7 @@
         <v>0.00642706</v>
       </c>
       <c r="Z51" s="26">
-        <v>0.00682379</v>
+        <v>0.008871804</v>
       </c>
       <c r="AA51" s="26">
         <v>0.0249992</v>
@@ -5373,7 +5373,7 @@
         <v>0.00634605</v>
       </c>
       <c r="Z52" s="26">
-        <v>0.00682379</v>
+        <v>0.008896932</v>
       </c>
       <c r="AA52" s="26">
         <v>0.0249992</v>
@@ -5462,7 +5462,7 @@
         <v>0.00720435</v>
       </c>
       <c r="Z53" s="26">
-        <v>0.00647584</v>
+        <v>0.009043237</v>
       </c>
       <c r="AA53" s="26">
         <v>0.02698983</v>
@@ -5551,7 +5551,7 @@
         <v>0.00797896</v>
       </c>
       <c r="Z54" s="26">
-        <v>0.00647584</v>
+        <v>0.007419152</v>
       </c>
       <c r="AA54" s="26">
         <v>0.02698983</v>
@@ -5640,7 +5640,7 @@
         <v>0.00681763</v>
       </c>
       <c r="Z55" s="26">
-        <v>0.00647584</v>
+        <v>0.005326929</v>
       </c>
       <c r="AA55" s="26">
         <v>0.02698983</v>
@@ -5729,7 +5729,7 @@
         <v>0.00541537</v>
       </c>
       <c r="Z56" s="26">
-        <v>0.00527329</v>
+        <v>0.005387444</v>
       </c>
       <c r="AA56" s="26">
         <v>0.02618672</v>
@@ -5818,7 +5818,7 @@
         <v>0.00858353</v>
       </c>
       <c r="Z57" s="26">
-        <v>0.00527329</v>
+        <v>0.005416423</v>
       </c>
       <c r="AA57" s="26">
         <v>0.02618672</v>
@@ -5907,7 +5907,7 @@
         <v>0.0087721</v>
       </c>
       <c r="Z58" s="26">
-        <v>0.00527329</v>
+        <v>0.005569252</v>
       </c>
       <c r="AA58" s="26">
         <v>0.02618672</v>
@@ -5996,7 +5996,7 @@
         <v>0.00898864</v>
       </c>
       <c r="Z59" s="26">
-        <v>0.00507377</v>
+        <v>0.005475777</v>
       </c>
       <c r="AA59" s="26">
         <v>0.02821883</v>
@@ -6085,7 +6085,7 @@
         <v>0.0090573</v>
       </c>
       <c r="Z60" s="26">
-        <v>0.00507377</v>
+        <v>0.006080188</v>
       </c>
       <c r="AA60" s="26">
         <v>0.02821883</v>
@@ -6174,7 +6174,7 @@
         <v>0.00926382</v>
       </c>
       <c r="Z61" s="26">
-        <v>0.00507377</v>
+        <v>0.006364543</v>
       </c>
       <c r="AA61" s="26">
         <v>0.02821883</v>
@@ -6263,7 +6263,7 @@
         <v>0.00961898</v>
       </c>
       <c r="Z62" s="26">
-        <v>0.00251595</v>
+        <v>0.005706014</v>
       </c>
       <c r="AA62" s="26">
         <v>0.02464009</v>
@@ -6352,7 +6352,7 @@
         <v>0.00904394</v>
       </c>
       <c r="Z63" s="26">
-        <v>0.00251595</v>
+        <v>0.005697494</v>
       </c>
       <c r="AA63" s="26">
         <v>0.02464009</v>
@@ -6441,7 +6441,7 @@
         <v>0.00705675</v>
       </c>
       <c r="Z64" s="26">
-        <v>0.00251595</v>
+        <v>0.005313886</v>
       </c>
       <c r="AA64" s="26">
         <v>0.02464009</v>
@@ -6530,7 +6530,7 @@
         <v>0.00777417</v>
       </c>
       <c r="Z65" s="26">
-        <v>0.00244619</v>
+        <v>0.004670057</v>
       </c>
       <c r="AA65" s="26">
         <v>0.01647761</v>
@@ -6619,7 +6619,7 @@
         <v>0.00835981</v>
       </c>
       <c r="Z66" s="26">
-        <v>0.00244619</v>
+        <v>0.004756537</v>
       </c>
       <c r="AA66" s="26">
         <v>0.01647761</v>
@@ -6708,7 +6708,7 @@
         <v>0.00625483</v>
       </c>
       <c r="Z67" s="26">
-        <v>0.00244619</v>
+        <v>0.004679792</v>
       </c>
       <c r="AA67" s="26">
         <v>0.01647761</v>
@@ -6797,7 +6797,7 @@
         <v>0.00558523</v>
       </c>
       <c r="Z68" s="26">
-        <v>0.00247921</v>
+        <v>0.004609429</v>
       </c>
       <c r="AA68" s="26">
         <v>0.01029606</v>
@@ -6886,7 +6886,7 @@
         <v>0.00583761</v>
       </c>
       <c r="Z69" s="26">
-        <v>0.00247921</v>
+        <v>0.004642215</v>
       </c>
       <c r="AA69" s="26">
         <v>0.01029606</v>
@@ -6975,7 +6975,7 @@
         <v>0.00559574</v>
       </c>
       <c r="Z70" s="26">
-        <v>0.00247921</v>
+        <v>0.004413638</v>
       </c>
       <c r="AA70" s="26">
         <v>0.01029606</v>
@@ -7064,7 +7064,7 @@
         <v>0.00532769</v>
       </c>
       <c r="Z71" s="26">
-        <v>0.00302709</v>
+        <v>0.004431792</v>
       </c>
       <c r="AA71" s="26">
         <v>0.00939885</v>
@@ -7153,7 +7153,7 @@
         <v>0.00514778</v>
       </c>
       <c r="Z72" s="26">
-        <v>0.00302709</v>
+        <v>0.003766553</v>
       </c>
       <c r="AA72" s="26">
         <v>0.00939885</v>
@@ -7242,7 +7242,7 @@
         <v>0.00530887</v>
       </c>
       <c r="Z73" s="26">
-        <v>0.00302709</v>
+        <v>0.003157921</v>
       </c>
       <c r="AA73" s="26">
         <v>0.00939885</v>
@@ -7331,7 +7331,7 @@
         <v>0.0053814</v>
       </c>
       <c r="Z74" s="26">
-        <v>0.00293808</v>
+        <v>0.003152868</v>
       </c>
       <c r="AA74" s="26">
         <v>0.0077348</v>
@@ -7420,7 +7420,7 @@
         <v>0.00575654</v>
       </c>
       <c r="Z75" s="26">
-        <v>0.00293808</v>
+        <v>0.0033333</v>
       </c>
       <c r="AA75" s="26">
         <v>0.0077348</v>
@@ -7509,7 +7509,7 @@
         <v>0.00701265</v>
       </c>
       <c r="Z76" s="26">
-        <v>0.00293808</v>
+        <v>0.003930282</v>
       </c>
       <c r="AA76" s="26">
         <v>0.0077348</v>
@@ -7598,7 +7598,7 @@
         <v>0.00672323</v>
       </c>
       <c r="Z77" s="26">
-        <v>0.00277094</v>
+        <v>0.005123196</v>
       </c>
       <c r="AA77" s="26">
         <v>0.00970477</v>
@@ -7687,7 +7687,7 @@
         <v>0.00621908</v>
       </c>
       <c r="Z78" s="26">
-        <v>0.00277094</v>
+        <v>0.004979118</v>
       </c>
       <c r="AA78" s="26">
         <v>0.00970477</v>
@@ -7776,7 +7776,7 @@
         <v>0.0075283</v>
       </c>
       <c r="Z79" s="26">
-        <v>0.00277094</v>
+        <v>0.00496894</v>
       </c>
       <c r="AA79" s="26">
         <v>0.00970477</v>
@@ -7865,7 +7865,7 @@
         <v>0.00685396</v>
       </c>
       <c r="Z80" s="26">
-        <v>0.00285459</v>
+        <v>0.004903979</v>
       </c>
       <c r="AA80" s="26">
         <v>0.00893429</v>
@@ -7954,7 +7954,7 @@
         <v>0.00566661</v>
       </c>
       <c r="Z81" s="26">
-        <v>0.00285459</v>
+        <v>0.004843456</v>
       </c>
       <c r="AA81" s="26">
         <v>0.00893429</v>
@@ -8043,7 +8043,7 @@
         <v>0.0061119</v>
       </c>
       <c r="Z82" s="26">
-        <v>0.00285459</v>
+        <v>0.004865316</v>
       </c>
       <c r="AA82" s="26">
         <v>0.00893429</v>
@@ -8132,7 +8132,7 @@
         <v>0.00600392</v>
       </c>
       <c r="Z83" s="26">
-        <v>0.00234587</v>
+        <v>0.004955363</v>
       </c>
       <c r="AA83" s="26">
         <v>0.01046523</v>
@@ -8221,7 +8221,7 @@
         <v>0.00596511</v>
       </c>
       <c r="Z84" s="26">
-        <v>0.00234587</v>
+        <v>0.004871904</v>
       </c>
       <c r="AA84" s="26">
         <v>0.01046523</v>
@@ -8310,7 +8310,7 @@
         <v>0.00595265</v>
       </c>
       <c r="Z85" s="26">
-        <v>0.00234587</v>
+        <v>0.004924779</v>
       </c>
       <c r="AA85" s="26">
         <v>0.01046523</v>
@@ -8399,7 +8399,7 @@
         <v>0.00562861</v>
       </c>
       <c r="Z86" s="26">
-        <v>0.00223536</v>
+        <v>0.004886225</v>
       </c>
       <c r="AA86" s="26">
         <v>0.01095419</v>
@@ -8488,7 +8488,7 @@
         <v>0.00611281</v>
       </c>
       <c r="Z87" s="26">
-        <v>0.00223536</v>
+        <v>0.004771036</v>
       </c>
       <c r="AA87" s="26">
         <v>0.01095419</v>
@@ -8577,7 +8577,7 @@
         <v>0.00642993</v>
       </c>
       <c r="Z88" s="26">
-        <v>0.00223536</v>
+        <v>0.004306355</v>
       </c>
       <c r="AA88" s="26">
         <v>0.01095419</v>
@@ -8666,7 +8666,7 @@
         <v>0.00617207</v>
       </c>
       <c r="Z89" s="26">
-        <v>0.0024171</v>
+        <v>0.002881445</v>
       </c>
       <c r="AA89" s="26">
         <v>0.02774416</v>
@@ -8755,7 +8755,7 @@
         <v>0.00594274</v>
       </c>
       <c r="Z90" s="26">
-        <v>0.00250927</v>
+        <v>0.002734998</v>
       </c>
       <c r="AA90" s="26">
         <v>0.02885347</v>

</xml_diff>